<commit_message>
Fixed bugged calculation, streamlined code, added custom tab
</commit_message>
<xml_diff>
--- a/rates.xlsx
+++ b/rates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
     <t>type</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>subtype</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -371,375 +365,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="C4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="C5">
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="C6">
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7">
+      <c r="C7">
         <v>0.94</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="C8">
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="C10">
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>3</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="C16">
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="D20">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="D21">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26">
+      <c r="C21">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>